<commit_message>
Mejora de modelo enriquesido y muestreo de datos residentes, exactamente residentes e inmuebles
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Residentes Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Residentes Muestreo Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69B8FC5-C25C-4C3F-85DC-A6317E7512F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEAED78-25CB-4083-A653-46662D85FCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A03FCC9F-8ADB-4317-A3D3-F6E5CE84BC70}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{A03FCC9F-8ADB-4317-A3D3-F6E5CE84BC70}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -248,9 +248,6 @@
     <t>apellido</t>
   </si>
   <si>
-    <t>tipoDeDocumento</t>
-  </si>
-  <si>
     <t>Es un dato que hace que cada inmueble sea único.</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>numeroContacto</t>
   </si>
   <si>
-    <t>correo</t>
-  </si>
-  <si>
     <t>Combinación única 2</t>
   </si>
   <si>
@@ -297,6 +291,12 @@
   </si>
   <si>
     <t>No puede haber mas de un residente con el mismo número de contacto</t>
+  </si>
+  <si>
+    <t>tipoDocumento</t>
+  </si>
+  <si>
+    <t>correoElectronico</t>
   </si>
 </sst>
 </file>
@@ -437,9 +437,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -451,6 +448,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -477,6 +477,41 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
+      <sheetName val="Valores"/>
+      <sheetName val="Modelo Dominio anémico contexto"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="Residente"/>
+      <sheetName val="Inmueble"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Objeto de dominio que representa a un residente que vive dentro de un inmueble en un conjunto residencial</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
       <sheetName val="Objetos de dominio"/>
       <sheetName val="Administrador"/>
       <sheetName val="ConjuntoResidencial"/>
@@ -485,9 +520,9 @@
       <sheetName val="ZonaComun"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="4">
           <cell r="E4" t="str">
@@ -530,43 +565,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Valores"/>
-      <sheetName val="Modelo Dominio anémico contexto"/>
-      <sheetName val="Listado Objetos de Dominio"/>
-      <sheetName val="Residente"/>
-      <sheetName val="Inmueble"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Objeto de dominio que representa a un residente que vive dentro de un inmueble en un conjunto residencial</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -891,7 +891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955E1381-9DD8-476B-8044-3E079F79E259}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -914,7 +914,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="str">
-        <f>'[2]Listado Objetos de Dominio'!$B$3</f>
+        <f>'[1]Listado Objetos de Dominio'!$B$3</f>
         <v>Objeto de dominio que representa a un residente que vive dentro de un inmueble en un conjunto residencial</v>
       </c>
     </row>
@@ -923,7 +923,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f>'[2]Listado Objetos de Dominio'!$B$4</f>
+        <f>'[1]Listado Objetos de Dominio'!$B$4</f>
         <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
       </c>
     </row>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74F213F-7D77-4A77-8569-EB0D1E5DC4A2}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,12 +959,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -972,45 +972,45 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:13" s="19" customFormat="1" ht="69" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:13" s="18" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K2" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" s="20" t="s">
+      <c r="K2" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="19" t="s">
         <v>82</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1024,19 +1024,19 @@
         <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
@@ -1048,10 +1048,10 @@
         <v>26</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1132,7 +1132,7 @@
         <v>Casa10 - Bloque1 - Forest apartamentos</v>
       </c>
       <c r="K5" s="13" t="str">
-        <f t="shared" ref="K5:M13" si="0">_xlfn.CONCAT(D5,"-",E5)</f>
+        <f t="shared" ref="K5:K13" si="0">_xlfn.CONCAT(D5,"-",E5)</f>
         <v>Registro civil-16513516</v>
       </c>
       <c r="L5" s="13">
@@ -1555,29 +1555,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1588,7 +1588,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>25</v>
@@ -1598,7 +1598,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1608,7 +1608,7 @@
         <v>102</v>
       </c>
       <c r="D4" s="2" t="str">
-        <f>[1]Zonainmueble!$E$4</f>
+        <f>[2]Zonainmueble!$E$4</f>
         <v>Torre1 - Forest apartamentos</v>
       </c>
       <c r="E4" s="15" t="str">
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1627,7 +1627,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f>[1]Zonainmueble!$E$5</f>
+        <f>[2]Zonainmueble!$E$5</f>
         <v>Bloque1 - Forest apartamentos</v>
       </c>
       <c r="E5" s="15" t="str">
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1646,7 +1646,7 @@
         <v>304</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f>[1]Zonainmueble!$E$6</f>
+        <f>[2]Zonainmueble!$E$6</f>
         <v>Torre2 - Forest apartamentos</v>
       </c>
       <c r="E6" s="15" t="str">
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1665,7 +1665,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f>[1]Zonainmueble!$E$7</f>
+        <f>[2]Zonainmueble!$E$7</f>
         <v>Bloque1 - Natural</v>
       </c>
       <c r="E7" s="15" t="str">
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1684,7 +1684,7 @@
         <v>423</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>[1]Zonainmueble!E10</f>
+        <f>[2]Zonainmueble!E10</f>
         <v>Bloque1 - Ventus</v>
       </c>
       <c r="E8" s="15" t="str">
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1703,7 +1703,7 @@
         <v>1204</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>[1]Zonainmueble!E11</f>
+        <f>[2]Zonainmueble!E11</f>
         <v>Torre1 - Bolivar</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="21">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1722,7 +1722,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>[1]Zonainmueble!E7</f>
+        <f>[2]Zonainmueble!E7</f>
         <v>Bloque1 - Natural</v>
       </c>
       <c r="E10" s="15" t="str">
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1741,7 +1741,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f>[1]Zonainmueble!E12</f>
+        <f>[2]Zonainmueble!E12</f>
         <v>Bloque2 - Riogrande</v>
       </c>
       <c r="E11" s="15" t="str">
@@ -1750,7 +1750,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="A12" s="21">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1760,7 +1760,7 @@
         <v>514</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>[1]Zonainmueble!E9</f>
+        <f>[2]Zonainmueble!E9</f>
         <v>Bloque1 - Riogrande</v>
       </c>
       <c r="E12" s="15" t="str">
@@ -1769,7 +1769,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1779,7 +1779,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="2" t="str">
-        <f>[1]Zonainmueble!E7</f>
+        <f>[2]Zonainmueble!E7</f>
         <v>Bloque1 - Natural</v>
       </c>
       <c r="E13" s="15" t="str">

</xml_diff>